<commit_message>
update sheet creation and line number
</commit_message>
<xml_diff>
--- a/planning/TestWriteTeachingUnits.xlsx
+++ b/planning/TestWriteTeachingUnits.xlsx
@@ -3985,7 +3985,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="24.0" customHeight="true"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="3" max="3" width="32.0" customWidth="true"/>
     <col min="2" max="2" width="32.0" customWidth="true"/>
@@ -4694,7 +4694,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="24.0" customHeight="true"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="3" max="3" width="32.0" customWidth="true"/>
     <col min="2" max="2" width="32.0" customWidth="true"/>

</xml_diff>